<commit_message>
Corrections et modification mineures
</commit_message>
<xml_diff>
--- a/RWEB/2025-06-Ref-eco_web-checklist.v5-en.xlsx
+++ b/RWEB/2025-06-Ref-eco_web-checklist.v5-en.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael.lemaire/Downloads/Checklist RWEB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael.lemaire/Documents/workspaces/CNumR/best-practices-checklists/RWEB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4403F400-A004-2748-9408-92A73B6BE146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B350C7C0-8B56-D148-86E3-263CB0C10990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="347">
   <si>
     <t>PO/AMOA</t>
   </si>
@@ -1135,12 +1135,15 @@
   <si>
     <t>Minifying text files: CSS, JS, HTML and SVG</t>
   </si>
+  <si>
+    <t>7. End of life</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1249,6 +1252,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1273,7 +1283,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -1329,6 +1339,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1616,14 +1629,14 @@
   </sheetPr>
   <dimension ref="A1:R117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="45.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="4.6640625" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="5.83203125" customWidth="1" outlineLevel="1"/>
     <col min="5" max="6" width="4.83203125" customWidth="1"/>
@@ -7029,8 +7042,8 @@
       <c r="G115" s="6">
         <v>4</v>
       </c>
-      <c r="H115" s="18" t="s">
-        <v>67</v>
+      <c r="H115" s="20" t="s">
+        <v>346</v>
       </c>
       <c r="I115" s="13" t="s">
         <v>72</v>
@@ -7077,8 +7090,8 @@
       <c r="G116" s="13">
         <v>3</v>
       </c>
-      <c r="H116" s="18" t="s">
-        <v>67</v>
+      <c r="H116" s="20" t="s">
+        <v>346</v>
       </c>
       <c r="I116" s="13" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Correction of v5 ids.
Actually, they changed in the v5 book.
</commit_message>
<xml_diff>
--- a/RWEB/2025-06-Ref-eco_web-checklist.v5-en.xlsx
+++ b/RWEB/2025-06-Ref-eco_web-checklist.v5-en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael.lemaire/Documents/workspaces/CNumR/best-practices-checklists/RWEB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B350C7C0-8B56-D148-86E3-263CB0C10990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33BE766-7A7B-8248-9DFE-8815EAA2AFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1629,8 +1629,8 @@
   </sheetPr>
   <dimension ref="A1:R117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:XFD102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
@@ -1650,7 +1650,7 @@
     <col min="17" max="17" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>55</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="6">
-        <f t="shared" ref="O3:O66" si="0">N3*G3</f>
+        <f t="shared" ref="O3:O67" si="0">N3*G3</f>
         <v>0</v>
       </c>
       <c r="P3" s="6"/>
@@ -3434,45 +3434,49 @@
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
     </row>
-    <row r="39" spans="1:17" ht="28" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="13" t="s">
-        <v>259</v>
+        <v>319</v>
       </c>
       <c r="B39" s="13">
-        <v>4038</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="13"/>
+        <v>161</v>
+      </c>
+      <c r="C39" s="7">
+        <v>21</v>
+      </c>
+      <c r="D39" s="13">
+        <v>35</v>
+      </c>
       <c r="E39" s="13">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="F39" s="13">
         <v>38</v>
       </c>
       <c r="G39" s="13">
-        <v>3</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="J39" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L39" s="7" t="s">
-        <v>105</v>
+      <c r="K39" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="L39" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="M39" s="12" t="s">
-        <v>148</v>
+        <v>208</v>
       </c>
       <c r="N39" s="6"/>
       <c r="O39" s="6">
-        <f t="shared" si="0"/>
+        <f>N39*G39</f>
         <v>0</v>
       </c>
       <c r="P39" s="6"/>
@@ -3480,19 +3484,15 @@
     </row>
     <row r="40" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B40" s="13">
-        <v>34</v>
-      </c>
-      <c r="C40" s="7">
-        <v>32</v>
-      </c>
-      <c r="D40" s="13">
-        <v>45</v>
-      </c>
+        <v>4038</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="13"/>
       <c r="E40" s="13">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F40" s="13">
         <v>39</v>
@@ -3516,7 +3516,7 @@
         <v>105</v>
       </c>
       <c r="M40" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N40" s="6"/>
       <c r="O40" s="6">
@@ -3528,19 +3528,19 @@
     </row>
     <row r="41" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B41" s="13">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C41" s="7">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D41" s="13">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E41" s="13">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F41" s="13">
         <v>40</v>
@@ -3564,7 +3564,7 @@
         <v>105</v>
       </c>
       <c r="M41" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N41" s="6"/>
       <c r="O41" s="6">
@@ -3576,25 +3576,25 @@
     </row>
     <row r="42" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B42" s="13">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C42" s="7">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D42" s="13">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E42" s="13">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F42" s="13">
         <v>41</v>
       </c>
       <c r="G42" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>65</v>
@@ -3606,13 +3606,13 @@
         <v>74</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L42" s="7" t="s">
         <v>105</v>
       </c>
       <c r="M42" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N42" s="6"/>
       <c r="O42" s="6">
@@ -3624,25 +3624,25 @@
     </row>
     <row r="43" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A43" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B43" s="13">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C43" s="7">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D43" s="13">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E43" s="13">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F43" s="13">
         <v>42</v>
       </c>
       <c r="G43" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>65</v>
@@ -3654,13 +3654,13 @@
         <v>74</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L43" s="7" t="s">
         <v>105</v>
       </c>
       <c r="M43" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N43" s="6"/>
       <c r="O43" s="6">
@@ -3672,25 +3672,25 @@
     </row>
     <row r="44" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A44" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B44" s="13">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C44" s="7">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D44" s="13">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E44" s="13">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F44" s="13">
         <v>43</v>
       </c>
       <c r="G44" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>65</v>
@@ -3702,13 +3702,13 @@
         <v>74</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L44" s="7" t="s">
         <v>105</v>
       </c>
       <c r="M44" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N44" s="6"/>
       <c r="O44" s="6">
@@ -3720,25 +3720,25 @@
     </row>
     <row r="45" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A45" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B45" s="13">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C45" s="7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45" s="13">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E45" s="13">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F45" s="13">
         <v>44</v>
       </c>
       <c r="G45" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H45" s="10" t="s">
         <v>65</v>
@@ -3756,7 +3756,7 @@
         <v>105</v>
       </c>
       <c r="M45" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N45" s="6"/>
       <c r="O45" s="6">
@@ -3768,15 +3768,19 @@
     </row>
     <row r="46" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A46" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B46" s="13">
-        <v>4045</v>
-      </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="13"/>
+        <v>44</v>
+      </c>
+      <c r="C46" s="7">
+        <v>44</v>
+      </c>
+      <c r="D46" s="13">
+        <v>42</v>
+      </c>
       <c r="E46" s="13">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F46" s="13">
         <v>45</v>
@@ -3793,14 +3797,14 @@
       <c r="J46" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K46" s="7" t="s">
-        <v>80</v>
+      <c r="K46" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="L46" s="7" t="s">
         <v>105</v>
       </c>
       <c r="M46" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N46" s="6"/>
       <c r="O46" s="6">
@@ -3812,19 +3816,15 @@
     </row>
     <row r="47" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A47" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B47" s="13">
-        <v>180</v>
-      </c>
-      <c r="C47" s="7">
-        <v>9</v>
-      </c>
-      <c r="D47" s="13">
-        <v>9</v>
-      </c>
+        <v>4045</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="13"/>
       <c r="E47" s="13">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F47" s="13">
         <v>46</v>
@@ -3841,14 +3841,14 @@
       <c r="J47" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K47" s="6" t="s">
-        <v>11</v>
+      <c r="K47" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="L47" s="7" t="s">
         <v>105</v>
       </c>
       <c r="M47" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N47" s="6"/>
       <c r="O47" s="6">
@@ -3860,25 +3860,25 @@
     </row>
     <row r="48" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B48" s="13">
-        <v>93</v>
+        <v>180</v>
       </c>
       <c r="C48" s="7">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D48" s="13">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E48" s="13">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F48" s="13">
         <v>47</v>
       </c>
       <c r="G48" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>65</v>
@@ -3889,14 +3889,14 @@
       <c r="J48" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K48" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="L48" s="13" t="s">
-        <v>107</v>
+      <c r="K48" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L48" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="M48" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N48" s="6"/>
       <c r="O48" s="6">
@@ -3908,25 +3908,25 @@
     </row>
     <row r="49" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A49" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B49" s="13">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="C49" s="7">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="D49" s="13">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="E49" s="13">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F49" s="13">
         <v>48</v>
       </c>
       <c r="G49" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H49" s="10" t="s">
         <v>65</v>
@@ -3944,7 +3944,7 @@
         <v>107</v>
       </c>
       <c r="M49" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N49" s="6"/>
       <c r="O49" s="6">
@@ -3956,19 +3956,19 @@
     </row>
     <row r="50" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A50" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B50" s="13">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C50" s="7">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="D50" s="13">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="E50" s="13">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F50" s="13">
         <v>49</v>
@@ -3989,10 +3989,10 @@
         <v>83</v>
       </c>
       <c r="L50" s="13" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="M50" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N50" s="6"/>
       <c r="O50" s="6">
@@ -4004,23 +4004,25 @@
     </row>
     <row r="51" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A51" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B51" s="13">
-        <v>1010</v>
-      </c>
-      <c r="C51" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="C51" s="7">
+        <v>18</v>
+      </c>
       <c r="D51" s="13">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E51" s="13">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F51" s="13">
         <v>50</v>
       </c>
       <c r="G51" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H51" s="10" t="s">
         <v>65</v>
@@ -4032,13 +4034,13 @@
         <v>74</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L51" s="13" t="s">
         <v>1</v>
       </c>
       <c r="M51" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N51" s="6"/>
       <c r="O51" s="6">
@@ -4050,19 +4052,17 @@
     </row>
     <row r="52" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A52" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B52" s="13">
-        <v>42</v>
-      </c>
-      <c r="C52" s="7">
-        <v>45</v>
-      </c>
+        <v>1010</v>
+      </c>
+      <c r="C52" s="7"/>
       <c r="D52" s="13">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E52" s="13">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F52" s="13">
         <v>51</v>
@@ -4079,14 +4079,14 @@
       <c r="J52" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K52" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L52" s="7" t="s">
-        <v>105</v>
+      <c r="K52" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L52" s="13" t="s">
+        <v>1</v>
       </c>
       <c r="M52" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N52" s="6"/>
       <c r="O52" s="6">
@@ -4097,22 +4097,26 @@
       <c r="Q52" s="6"/>
     </row>
     <row r="53" spans="1:17" ht="28" x14ac:dyDescent="0.15">
-      <c r="A53" s="12" t="s">
-        <v>273</v>
+      <c r="A53" s="13" t="s">
+        <v>272</v>
       </c>
       <c r="B53" s="13">
-        <v>4052</v>
-      </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="13"/>
+        <v>42</v>
+      </c>
+      <c r="C53" s="7">
+        <v>45</v>
+      </c>
+      <c r="D53" s="13">
+        <v>43</v>
+      </c>
       <c r="E53" s="13">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F53" s="13">
         <v>52</v>
       </c>
       <c r="G53" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H53" s="10" t="s">
         <v>65</v>
@@ -4130,7 +4134,7 @@
         <v>105</v>
       </c>
       <c r="M53" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N53" s="6"/>
       <c r="O53" s="6">
@@ -4141,20 +4145,16 @@
       <c r="Q53" s="6"/>
     </row>
     <row r="54" spans="1:17" ht="28" x14ac:dyDescent="0.15">
-      <c r="A54" s="13" t="s">
-        <v>274</v>
+      <c r="A54" s="12" t="s">
+        <v>273</v>
       </c>
       <c r="B54" s="13">
-        <v>33</v>
-      </c>
-      <c r="C54" s="7">
-        <v>36</v>
-      </c>
-      <c r="D54" s="13">
-        <v>49</v>
-      </c>
+        <v>4052</v>
+      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="13"/>
       <c r="E54" s="13">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F54" s="13">
         <v>53</v>
@@ -4178,7 +4178,7 @@
         <v>105</v>
       </c>
       <c r="M54" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N54" s="6"/>
       <c r="O54" s="6">
@@ -4190,21 +4190,25 @@
     </row>
     <row r="55" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A55" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B55" s="13">
-        <v>4054</v>
-      </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="C55" s="7">
+        <v>36</v>
+      </c>
+      <c r="D55" s="13">
+        <v>49</v>
+      </c>
       <c r="E55" s="13">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F55" s="13">
         <v>54</v>
       </c>
       <c r="G55" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H55" s="10" t="s">
         <v>65</v>
@@ -4222,7 +4226,7 @@
         <v>105</v>
       </c>
       <c r="M55" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N55" s="6"/>
       <c r="O55" s="6">
@@ -4234,25 +4238,21 @@
     </row>
     <row r="56" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A56" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B56" s="13">
-        <v>41</v>
-      </c>
-      <c r="C56" s="7">
-        <v>46</v>
-      </c>
-      <c r="D56" s="13">
-        <v>44</v>
-      </c>
+        <v>4054</v>
+      </c>
+      <c r="C56" s="7"/>
+      <c r="D56" s="13"/>
       <c r="E56" s="13">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F56" s="13">
         <v>55</v>
       </c>
       <c r="G56" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H56" s="10" t="s">
         <v>65</v>
@@ -4270,7 +4270,7 @@
         <v>105</v>
       </c>
       <c r="M56" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N56" s="6"/>
       <c r="O56" s="6">
@@ -4282,25 +4282,25 @@
     </row>
     <row r="57" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A57" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B57" s="13">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C57" s="7">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D57" s="13">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E57" s="13">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F57" s="13">
         <v>56</v>
       </c>
       <c r="G57" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H57" s="10" t="s">
         <v>65</v>
@@ -4318,7 +4318,7 @@
         <v>105</v>
       </c>
       <c r="M57" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N57" s="6"/>
       <c r="O57" s="6">
@@ -4330,21 +4330,25 @@
     </row>
     <row r="58" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A58" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B58" s="13">
-        <v>4057</v>
-      </c>
-      <c r="C58" s="7"/>
-      <c r="D58" s="13"/>
+        <v>32</v>
+      </c>
+      <c r="C58" s="7">
+        <v>42</v>
+      </c>
+      <c r="D58" s="13">
+        <v>54</v>
+      </c>
       <c r="E58" s="13">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F58" s="13">
         <v>57</v>
       </c>
       <c r="G58" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H58" s="10" t="s">
         <v>65</v>
@@ -4355,14 +4359,14 @@
       <c r="J58" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K58" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="L58" s="13" t="s">
-        <v>104</v>
+      <c r="K58" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L58" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="M58" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N58" s="6"/>
       <c r="O58" s="6">
@@ -4374,23 +4378,21 @@
     </row>
     <row r="59" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A59" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B59" s="13">
-        <v>910</v>
+        <v>4057</v>
       </c>
       <c r="C59" s="7"/>
-      <c r="D59" s="13">
-        <v>19</v>
-      </c>
+      <c r="D59" s="13"/>
       <c r="E59" s="13">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F59" s="13">
         <v>58</v>
       </c>
       <c r="G59" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H59" s="10" t="s">
         <v>65</v>
@@ -4402,13 +4404,13 @@
         <v>74</v>
       </c>
       <c r="K59" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L59" s="13" t="s">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="M59" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N59" s="6"/>
       <c r="O59" s="6">
@@ -4419,22 +4421,24 @@
       <c r="Q59" s="6"/>
     </row>
     <row r="60" spans="1:17" ht="28" x14ac:dyDescent="0.15">
-      <c r="A60" s="12" t="s">
-        <v>280</v>
+      <c r="A60" s="13" t="s">
+        <v>279</v>
       </c>
       <c r="B60" s="13">
-        <v>4059</v>
+        <v>910</v>
       </c>
       <c r="C60" s="7"/>
-      <c r="D60" s="13"/>
+      <c r="D60" s="13">
+        <v>19</v>
+      </c>
       <c r="E60" s="13">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F60" s="13">
         <v>59</v>
       </c>
       <c r="G60" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H60" s="10" t="s">
         <v>65</v>
@@ -4446,13 +4450,13 @@
         <v>74</v>
       </c>
       <c r="K60" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="L60" s="7" t="s">
-        <v>105</v>
+        <v>86</v>
+      </c>
+      <c r="L60" s="13" t="s">
+        <v>1</v>
       </c>
       <c r="M60" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N60" s="6"/>
       <c r="O60" s="6">
@@ -4463,26 +4467,22 @@
       <c r="Q60" s="6"/>
     </row>
     <row r="61" spans="1:17" ht="28" x14ac:dyDescent="0.15">
-      <c r="A61" s="13" t="s">
-        <v>281</v>
+      <c r="A61" s="12" t="s">
+        <v>280</v>
       </c>
       <c r="B61" s="13">
-        <v>8</v>
-      </c>
-      <c r="C61" s="7">
-        <v>15</v>
-      </c>
-      <c r="D61" s="13">
-        <v>31</v>
-      </c>
+        <v>4059</v>
+      </c>
+      <c r="C61" s="7"/>
+      <c r="D61" s="13"/>
       <c r="E61" s="13">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F61" s="13">
         <v>60</v>
       </c>
       <c r="G61" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>65</v>
@@ -4493,14 +4493,14 @@
       <c r="J61" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K61" s="6" t="s">
-        <v>16</v>
+      <c r="K61" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="L61" s="7" t="s">
         <v>105</v>
       </c>
       <c r="M61" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N61" s="6"/>
       <c r="O61" s="6">
@@ -4512,43 +4512,43 @@
     </row>
     <row r="62" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A62" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B62" s="13">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="C62" s="7">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="D62" s="13">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="E62" s="13">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F62" s="13">
         <v>61</v>
       </c>
       <c r="G62" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H62" s="10" t="s">
         <v>65</v>
       </c>
       <c r="I62" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J62" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K62" s="7" t="s">
-        <v>88</v>
+      <c r="K62" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="L62" s="7" t="s">
         <v>105</v>
       </c>
       <c r="M62" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N62" s="6"/>
       <c r="O62" s="6">
@@ -4560,19 +4560,19 @@
     </row>
     <row r="63" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A63" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B63" s="13">
-        <v>113</v>
+        <v>65</v>
       </c>
       <c r="C63" s="7">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="D63" s="13">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="E63" s="13">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F63" s="13">
         <v>62</v>
@@ -4590,13 +4590,13 @@
         <v>74</v>
       </c>
       <c r="K63" s="7" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="L63" s="7" t="s">
         <v>105</v>
       </c>
       <c r="M63" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N63" s="6"/>
       <c r="O63" s="6">
@@ -4608,19 +4608,19 @@
     </row>
     <row r="64" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A64" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B64" s="13">
-        <v>205</v>
+        <v>113</v>
       </c>
       <c r="C64" s="7">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="D64" s="13">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E64" s="13">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F64" s="13">
         <v>63</v>
@@ -4644,7 +4644,7 @@
         <v>105</v>
       </c>
       <c r="M64" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N64" s="6"/>
       <c r="O64" s="6">
@@ -4656,25 +4656,25 @@
     </row>
     <row r="65" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A65" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B65" s="13">
-        <v>55</v>
+        <v>205</v>
       </c>
       <c r="C65" s="7">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="D65" s="13">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="E65" s="13">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F65" s="13">
         <v>64</v>
       </c>
       <c r="G65" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H65" s="10" t="s">
         <v>65</v>
@@ -4686,13 +4686,13 @@
         <v>74</v>
       </c>
       <c r="K65" s="7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="L65" s="7" t="s">
         <v>105</v>
       </c>
       <c r="M65" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N65" s="6"/>
       <c r="O65" s="6">
@@ -4704,19 +4704,19 @@
     </row>
     <row r="66" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A66" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B66" s="13">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C66" s="7">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D66" s="13">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E66" s="13">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F66" s="13">
         <v>65</v>
@@ -4740,7 +4740,7 @@
         <v>105</v>
       </c>
       <c r="M66" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N66" s="6"/>
       <c r="O66" s="6">
@@ -4750,27 +4750,27 @@
       <c r="P66" s="6"/>
       <c r="Q66" s="6"/>
     </row>
-    <row r="67" spans="1:17" ht="42" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A67" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B67" s="13">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C67" s="7">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="D67" s="13">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="E67" s="13">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F67" s="13">
         <v>66</v>
       </c>
       <c r="G67" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H67" s="10" t="s">
         <v>65</v>
@@ -4782,17 +4782,17 @@
         <v>74</v>
       </c>
       <c r="K67" s="7" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="L67" s="7" t="s">
         <v>105</v>
       </c>
       <c r="M67" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N67" s="6"/>
       <c r="O67" s="6">
-        <f t="shared" ref="O67:O116" si="1">N67*G67</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P67" s="6"/>
@@ -4800,25 +4800,25 @@
     </row>
     <row r="68" spans="1:17" ht="42" x14ac:dyDescent="0.15">
       <c r="A68" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B68" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C68" s="7">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="D68" s="13">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E68" s="13">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F68" s="13">
         <v>67</v>
       </c>
       <c r="G68" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H68" s="10" t="s">
         <v>65</v>
@@ -4836,32 +4836,36 @@
         <v>105</v>
       </c>
       <c r="M68" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N68" s="6"/>
       <c r="O68" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="O68:O116" si="1">N68*G68</f>
         <v>0</v>
       </c>
       <c r="P68" s="6"/>
       <c r="Q68" s="6"/>
     </row>
-    <row r="69" spans="1:17" ht="28" x14ac:dyDescent="0.15">
-      <c r="A69" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="B69" s="6">
-        <v>4068</v>
-      </c>
-      <c r="C69" s="7"/>
-      <c r="D69" s="6"/>
+    <row r="69" spans="1:17" ht="42" x14ac:dyDescent="0.15">
+      <c r="A69" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="B69" s="13">
+        <v>4</v>
+      </c>
+      <c r="C69" s="7">
+        <v>53</v>
+      </c>
+      <c r="D69" s="13">
+        <v>16</v>
+      </c>
       <c r="E69" s="13">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F69" s="13">
         <v>68</v>
       </c>
-      <c r="G69" s="6">
+      <c r="G69" s="13">
         <v>3</v>
       </c>
       <c r="H69" s="10" t="s">
@@ -4874,13 +4878,13 @@
         <v>74</v>
       </c>
       <c r="K69" s="7" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M69" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N69" s="6"/>
       <c r="O69" s="6">
@@ -4891,44 +4895,40 @@
       <c r="Q69" s="6"/>
     </row>
     <row r="70" spans="1:17" ht="28" x14ac:dyDescent="0.15">
-      <c r="A70" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="B70" s="13">
-        <v>75</v>
-      </c>
-      <c r="C70" s="7">
-        <v>102</v>
-      </c>
-      <c r="D70" s="13">
-        <v>98</v>
-      </c>
+      <c r="A70" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B70" s="6">
+        <v>4068</v>
+      </c>
+      <c r="C70" s="7"/>
+      <c r="D70" s="6"/>
       <c r="E70" s="13">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F70" s="13">
         <v>69</v>
       </c>
-      <c r="G70" s="13">
-        <v>4</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="I70" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J70" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K70" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L70" s="13" t="s">
-        <v>109</v>
+      <c r="G70" s="6">
+        <v>3</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I70" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J70" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="K70" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L70" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="M70" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N70" s="6"/>
       <c r="O70" s="6">
@@ -4940,19 +4940,19 @@
     </row>
     <row r="71" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A71" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B71" s="13">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C71" s="7">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="D71" s="13">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="E71" s="13">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F71" s="13">
         <v>70</v>
@@ -4970,13 +4970,13 @@
         <v>31</v>
       </c>
       <c r="K71" s="6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="L71" s="13" t="s">
         <v>109</v>
       </c>
       <c r="M71" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N71" s="6"/>
       <c r="O71" s="6">
@@ -4988,25 +4988,25 @@
     </row>
     <row r="72" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A72" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B72" s="13">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="C72" s="7">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="D72" s="13">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="E72" s="13">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F72" s="13">
         <v>71</v>
       </c>
       <c r="G72" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H72" s="16" t="s">
         <v>2</v>
@@ -5017,14 +5017,14 @@
       <c r="J72" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="K72" s="7" t="s">
-        <v>101</v>
+      <c r="K72" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="L72" s="13" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="M72" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N72" s="6"/>
       <c r="O72" s="6">
@@ -5036,19 +5036,19 @@
     </row>
     <row r="73" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A73" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B73" s="13">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C73" s="7">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="D73" s="13">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E73" s="13">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F73" s="13">
         <v>72</v>
@@ -5069,10 +5069,10 @@
         <v>101</v>
       </c>
       <c r="L73" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M73" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N73" s="6"/>
       <c r="O73" s="6">
@@ -5084,25 +5084,25 @@
     </row>
     <row r="74" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A74" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B74" s="13">
+        <v>85</v>
+      </c>
+      <c r="C74" s="7">
+        <v>90</v>
+      </c>
+      <c r="D74" s="13">
+        <v>92</v>
+      </c>
+      <c r="E74" s="13">
         <v>72</v>
-      </c>
-      <c r="C74" s="7">
-        <v>103</v>
-      </c>
-      <c r="D74" s="13">
-        <v>99</v>
-      </c>
-      <c r="E74" s="13">
-        <v>73</v>
       </c>
       <c r="F74" s="13">
         <v>73</v>
       </c>
       <c r="G74" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H74" s="16" t="s">
         <v>2</v>
@@ -5114,13 +5114,13 @@
         <v>31</v>
       </c>
       <c r="K74" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L74" s="13" t="s">
         <v>109</v>
       </c>
       <c r="M74" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N74" s="6"/>
       <c r="O74" s="6">
@@ -5132,19 +5132,19 @@
     </row>
     <row r="75" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A75" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B75" s="13">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C75" s="7">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D75" s="13">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E75" s="13">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F75" s="13">
         <v>74</v>
@@ -5168,7 +5168,7 @@
         <v>109</v>
       </c>
       <c r="M75" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N75" s="6"/>
       <c r="O75" s="6">
@@ -5180,19 +5180,19 @@
     </row>
     <row r="76" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A76" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B76" s="13">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C76" s="7">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="D76" s="13">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="E76" s="13">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F76" s="13">
         <v>75</v>
@@ -5206,17 +5206,17 @@
       <c r="I76" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J76" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="K76" s="6" t="s">
-        <v>6</v>
+      <c r="J76" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K76" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="L76" s="13" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="M76" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N76" s="6"/>
       <c r="O76" s="6">
@@ -5324,15 +5324,19 @@
     </row>
     <row r="79" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A79" s="13" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B79" s="13">
-        <v>4078</v>
-      </c>
-      <c r="C79" s="7"/>
-      <c r="D79" s="13"/>
+        <v>89</v>
+      </c>
+      <c r="C79" s="7">
+        <v>81</v>
+      </c>
+      <c r="D79" s="13">
+        <v>79</v>
+      </c>
       <c r="E79" s="13">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F79" s="13">
         <v>78</v>
@@ -5346,21 +5350,21 @@
       <c r="I79" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J79" s="12" t="s">
+      <c r="J79" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="K79" s="7" t="s">
-        <v>80</v>
+      <c r="K79" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="L79" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M79" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="N79" s="6"/>
       <c r="O79" s="6">
-        <f t="shared" si="1"/>
+        <f>N79*G79</f>
         <v>0</v>
       </c>
       <c r="P79" s="6"/>
@@ -5368,25 +5372,21 @@
     </row>
     <row r="80" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A80" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B80" s="13">
-        <v>71</v>
-      </c>
-      <c r="C80" s="7">
-        <v>92</v>
-      </c>
-      <c r="D80" s="13">
-        <v>93</v>
-      </c>
+        <v>4078</v>
+      </c>
+      <c r="C80" s="7"/>
+      <c r="D80" s="13"/>
       <c r="E80" s="13">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F80" s="13">
         <v>79</v>
       </c>
       <c r="G80" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H80" s="16" t="s">
         <v>2</v>
@@ -5404,7 +5404,7 @@
         <v>109</v>
       </c>
       <c r="M80" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N80" s="6"/>
       <c r="O80" s="6">
@@ -5416,25 +5416,25 @@
     </row>
     <row r="81" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A81" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B81" s="13">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C81" s="7">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D81" s="13">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E81" s="13">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F81" s="13">
         <v>80</v>
       </c>
       <c r="G81" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H81" s="16" t="s">
         <v>2</v>
@@ -5442,11 +5442,11 @@
       <c r="I81" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J81" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="K81" s="6" t="s">
-        <v>6</v>
+      <c r="J81" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K81" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="L81" s="13" t="s">
         <v>109</v>
@@ -5464,25 +5464,25 @@
     </row>
     <row r="82" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A82" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B82" s="13">
-        <v>170</v>
+        <v>73</v>
       </c>
       <c r="C82" s="7">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="D82" s="13">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="E82" s="13">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F82" s="13">
         <v>81</v>
       </c>
       <c r="G82" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H82" s="16" t="s">
         <v>2</v>
@@ -5490,17 +5490,17 @@
       <c r="I82" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J82" s="12" t="s">
+      <c r="J82" s="13" t="s">
         <v>77</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="L82" s="13" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="M82" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N82" s="6"/>
       <c r="O82" s="6">
@@ -5512,21 +5512,25 @@
     </row>
     <row r="83" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A83" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B83" s="13">
-        <v>4082</v>
-      </c>
-      <c r="C83" s="7"/>
-      <c r="D83" s="13"/>
+        <v>170</v>
+      </c>
+      <c r="C83" s="7">
+        <v>55</v>
+      </c>
+      <c r="D83" s="13">
+        <v>18</v>
+      </c>
       <c r="E83" s="13">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F83" s="13">
         <v>82</v>
       </c>
       <c r="G83" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H83" s="16" t="s">
         <v>2</v>
@@ -5537,14 +5541,14 @@
       <c r="J83" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="K83" s="7" t="s">
-        <v>103</v>
+      <c r="K83" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="L83" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M83" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N83" s="6"/>
       <c r="O83" s="6">
@@ -5556,25 +5560,21 @@
     </row>
     <row r="84" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A84" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B84" s="13">
-        <v>1060</v>
-      </c>
-      <c r="C84" s="7">
-        <v>84</v>
-      </c>
-      <c r="D84" s="13">
-        <v>84</v>
-      </c>
+        <v>4082</v>
+      </c>
+      <c r="C84" s="7"/>
+      <c r="D84" s="13"/>
       <c r="E84" s="13">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F84" s="13">
         <v>83</v>
       </c>
       <c r="G84" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H84" s="16" t="s">
         <v>2</v>
@@ -5592,7 +5592,7 @@
         <v>109</v>
       </c>
       <c r="M84" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N84" s="6"/>
       <c r="O84" s="6">
@@ -5604,25 +5604,25 @@
     </row>
     <row r="85" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A85" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B85" s="13">
+        <v>1060</v>
+      </c>
+      <c r="C85" s="7">
         <v>84</v>
       </c>
-      <c r="C85" s="7">
-        <v>100</v>
-      </c>
       <c r="D85" s="13">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="E85" s="13">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F85" s="13">
         <v>84</v>
       </c>
       <c r="G85" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H85" s="16" t="s">
         <v>2</v>
@@ -5640,7 +5640,7 @@
         <v>109</v>
       </c>
       <c r="M85" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N85" s="6"/>
       <c r="O85" s="6">
@@ -5652,19 +5652,19 @@
     </row>
     <row r="86" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A86" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B86" s="13">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C86" s="7">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D86" s="13">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E86" s="13">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F86" s="13">
         <v>85</v>
@@ -5678,17 +5678,17 @@
       <c r="I86" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J86" s="13" t="s">
-        <v>78</v>
+      <c r="J86" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="K86" s="7" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="L86" s="13" t="s">
         <v>109</v>
       </c>
       <c r="M86" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N86" s="6"/>
       <c r="O86" s="6">
@@ -5700,19 +5700,19 @@
     </row>
     <row r="87" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A87" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B87" s="13">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C87" s="7">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D87" s="13">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E87" s="13">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F87" s="13">
         <v>86</v>
@@ -5726,17 +5726,17 @@
       <c r="I87" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J87" s="12" t="s">
+      <c r="J87" s="13" t="s">
         <v>78</v>
       </c>
       <c r="K87" s="7" t="s">
         <v>90</v>
       </c>
       <c r="L87" s="13" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="M87" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N87" s="6"/>
       <c r="O87" s="6">
@@ -5748,19 +5748,19 @@
     </row>
     <row r="88" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A88" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B88" s="13">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="C88" s="7">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="D88" s="13">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="E88" s="13">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F88" s="13">
         <v>87</v>
@@ -5781,10 +5781,10 @@
         <v>90</v>
       </c>
       <c r="L88" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M88" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N88" s="6"/>
       <c r="O88" s="6">
@@ -5796,19 +5796,19 @@
     </row>
     <row r="89" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A89" s="13" t="s">
-        <v>344</v>
+        <v>307</v>
       </c>
       <c r="B89" s="13">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="C89" s="7">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="D89" s="13">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="E89" s="13">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F89" s="13">
         <v>88</v>
@@ -5826,13 +5826,13 @@
         <v>78</v>
       </c>
       <c r="K89" s="7" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="L89" s="13" t="s">
         <v>109</v>
       </c>
       <c r="M89" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N89" s="6"/>
       <c r="O89" s="6">
@@ -5844,15 +5844,19 @@
     </row>
     <row r="90" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A90" s="13" t="s">
-        <v>308</v>
+        <v>344</v>
       </c>
       <c r="B90" s="13">
-        <v>4089</v>
-      </c>
-      <c r="C90" s="7"/>
-      <c r="D90" s="13"/>
+        <v>81</v>
+      </c>
+      <c r="C90" s="7">
+        <v>101</v>
+      </c>
+      <c r="D90" s="13">
+        <v>105</v>
+      </c>
       <c r="E90" s="13">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F90" s="13">
         <v>89</v>
@@ -5870,13 +5874,13 @@
         <v>78</v>
       </c>
       <c r="K90" s="7" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="L90" s="13" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="M90" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N90" s="6"/>
       <c r="O90" s="6">
@@ -5888,19 +5892,15 @@
     </row>
     <row r="91" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A91" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B91" s="13">
-        <v>501</v>
-      </c>
-      <c r="C91" s="7">
-        <v>86</v>
-      </c>
-      <c r="D91" s="13">
-        <v>88</v>
-      </c>
+        <v>4089</v>
+      </c>
+      <c r="C91" s="7"/>
+      <c r="D91" s="13"/>
       <c r="E91" s="13">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F91" s="13">
         <v>90</v>
@@ -5914,17 +5914,17 @@
       <c r="I91" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J91" s="13" t="s">
-        <v>79</v>
+      <c r="J91" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="K91" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L91" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M91" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N91" s="6"/>
       <c r="O91" s="6">
@@ -5934,21 +5934,21 @@
       <c r="P91" s="6"/>
       <c r="Q91" s="6"/>
     </row>
-    <row r="92" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A92" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B92" s="13">
-        <v>70</v>
+        <v>501</v>
       </c>
       <c r="C92" s="7">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D92" s="13">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E92" s="13">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F92" s="13">
         <v>91</v>
@@ -5960,19 +5960,19 @@
         <v>2</v>
       </c>
       <c r="I92" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J92" s="12" t="s">
-        <v>78</v>
+        <v>28</v>
+      </c>
+      <c r="J92" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="K92" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="L92" s="13" t="s">
         <v>109</v>
       </c>
       <c r="M92" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N92" s="6"/>
       <c r="O92" s="6">
@@ -5982,21 +5982,21 @@
       <c r="P92" s="6"/>
       <c r="Q92" s="6"/>
     </row>
-    <row r="93" spans="1:17" ht="28" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A93" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B93" s="13">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C93" s="7">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D93" s="13">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E93" s="13">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F93" s="13">
         <v>92</v>
@@ -6020,7 +6020,7 @@
         <v>109</v>
       </c>
       <c r="M93" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N93" s="6"/>
       <c r="O93" s="6">
@@ -6030,27 +6030,27 @@
       <c r="P93" s="6"/>
       <c r="Q93" s="6"/>
     </row>
-    <row r="94" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A94" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B94" s="13">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C94" s="7">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D94" s="13">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E94" s="13">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F94" s="13">
         <v>93</v>
       </c>
       <c r="G94" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H94" s="16" t="s">
         <v>2</v>
@@ -6068,7 +6068,7 @@
         <v>109</v>
       </c>
       <c r="M94" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N94" s="6"/>
       <c r="O94" s="6">
@@ -6078,27 +6078,27 @@
       <c r="P94" s="6"/>
       <c r="Q94" s="6"/>
     </row>
-    <row r="95" spans="1:17" ht="28" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B95" s="13">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C95" s="7">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D95" s="13">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E95" s="13">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F95" s="13">
         <v>94</v>
       </c>
       <c r="G95" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H95" s="16" t="s">
         <v>2</v>
@@ -6107,16 +6107,16 @@
         <v>68</v>
       </c>
       <c r="J95" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K95" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="L95" s="13" t="s">
         <v>109</v>
       </c>
       <c r="M95" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N95" s="6"/>
       <c r="O95" s="6">
@@ -6126,21 +6126,21 @@
       <c r="P95" s="6"/>
       <c r="Q95" s="6"/>
     </row>
-    <row r="96" spans="1:17" ht="14" x14ac:dyDescent="0.15">
-      <c r="A96" s="12" t="s">
-        <v>314</v>
+    <row r="96" spans="1:17" ht="28" x14ac:dyDescent="0.15">
+      <c r="A96" s="13" t="s">
+        <v>313</v>
       </c>
       <c r="B96" s="13">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C96" s="7">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D96" s="13">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E96" s="13">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F96" s="13">
         <v>95</v>
@@ -6158,13 +6158,13 @@
         <v>79</v>
       </c>
       <c r="K96" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L96" s="13" t="s">
         <v>109</v>
       </c>
       <c r="M96" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N96" s="6"/>
       <c r="O96" s="6">
@@ -6175,23 +6175,25 @@
       <c r="Q96" s="6"/>
     </row>
     <row r="97" spans="1:17" ht="14" x14ac:dyDescent="0.15">
-      <c r="A97" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="B97" s="6">
-        <v>4096</v>
-      </c>
-      <c r="C97" s="7"/>
-      <c r="D97" s="6">
-        <v>0</v>
+      <c r="A97" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="B97" s="13">
+        <v>66</v>
+      </c>
+      <c r="C97" s="7">
+        <v>84</v>
+      </c>
+      <c r="D97" s="13">
+        <v>86</v>
       </c>
       <c r="E97" s="13">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F97" s="13">
         <v>96</v>
       </c>
-      <c r="G97" s="6">
+      <c r="G97" s="13">
         <v>3</v>
       </c>
       <c r="H97" s="16" t="s">
@@ -6210,7 +6212,7 @@
         <v>109</v>
       </c>
       <c r="M97" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N97" s="6"/>
       <c r="O97" s="6">
@@ -6220,45 +6222,43 @@
       <c r="P97" s="6"/>
       <c r="Q97" s="6"/>
     </row>
-    <row r="98" spans="1:17" ht="28" x14ac:dyDescent="0.15">
-      <c r="A98" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="B98" s="13">
-        <v>99</v>
-      </c>
-      <c r="C98" s="7">
-        <v>58</v>
-      </c>
-      <c r="D98" s="13">
-        <v>58</v>
+    <row r="98" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+      <c r="A98" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B98" s="6">
+        <v>4096</v>
+      </c>
+      <c r="C98" s="7"/>
+      <c r="D98" s="6">
+        <v>0</v>
       </c>
       <c r="E98" s="13">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F98" s="13">
         <v>97</v>
       </c>
-      <c r="G98" s="13">
-        <v>5</v>
-      </c>
-      <c r="H98" s="17" t="s">
-        <v>66</v>
+      <c r="G98" s="6">
+        <v>3</v>
+      </c>
+      <c r="H98" s="16" t="s">
+        <v>2</v>
       </c>
       <c r="I98" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="J98" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="K98" s="6" t="s">
-        <v>7</v>
+        <v>68</v>
+      </c>
+      <c r="J98" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="K98" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="L98" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M98" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N98" s="6"/>
       <c r="O98" s="6">
@@ -6268,23 +6268,27 @@
       <c r="P98" s="6"/>
       <c r="Q98" s="6"/>
     </row>
-    <row r="99" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A99" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B99" s="13">
-        <v>4098</v>
-      </c>
-      <c r="C99" s="7"/>
-      <c r="D99" s="13"/>
+        <v>99</v>
+      </c>
+      <c r="C99" s="7">
+        <v>58</v>
+      </c>
+      <c r="D99" s="13">
+        <v>58</v>
+      </c>
       <c r="E99" s="13">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F99" s="13">
         <v>98</v>
       </c>
       <c r="G99" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H99" s="17" t="s">
         <v>66</v>
@@ -6295,14 +6299,14 @@
       <c r="J99" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K99" s="7" t="s">
-        <v>96</v>
+      <c r="K99" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="L99" s="13" t="s">
         <v>107</v>
       </c>
       <c r="M99" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N99" s="6"/>
       <c r="O99" s="6">
@@ -6314,25 +6318,21 @@
     </row>
     <row r="100" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A100" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B100" s="13">
-        <v>1050</v>
-      </c>
-      <c r="C100" s="7">
-        <v>22</v>
-      </c>
-      <c r="D100" s="13">
-        <v>36</v>
-      </c>
+        <v>4098</v>
+      </c>
+      <c r="C100" s="7"/>
+      <c r="D100" s="13"/>
       <c r="E100" s="13">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F100" s="13">
         <v>99</v>
       </c>
       <c r="G100" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H100" s="17" t="s">
         <v>66</v>
@@ -6350,7 +6350,7 @@
         <v>107</v>
       </c>
       <c r="M100" s="12" t="s">
-        <v>158</v>
+        <v>207</v>
       </c>
       <c r="N100" s="6"/>
       <c r="O100" s="6">
@@ -6362,25 +6362,25 @@
     </row>
     <row r="101" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A101" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B101" s="13">
-        <v>161</v>
+        <v>1050</v>
       </c>
       <c r="C101" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D101" s="13">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E101" s="13">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F101" s="13">
         <v>100</v>
       </c>
       <c r="G101" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H101" s="17" t="s">
         <v>66</v>
@@ -6398,7 +6398,7 @@
         <v>107</v>
       </c>
       <c r="M101" s="12" t="s">
-        <v>208</v>
+        <v>158</v>
       </c>
       <c r="N101" s="6"/>
       <c r="O101" s="6">

</xml_diff>